<commit_message>
progress bar fixed 2
</commit_message>
<xml_diff>
--- a/temp_data.xlsx
+++ b/temp_data.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BonpetData" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -431,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -448,6 +449,11 @@
           <t>АВР-Б-100-2-1</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>87 900 ₽</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -455,11 +461,21 @@
           <t>bababab</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Не найдено</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>267515</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>105 678 ₽</t>
         </is>
       </c>
     </row>
@@ -467,4 +483,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>АВР-Б-100-2-1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>87 900 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>bababab</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Не найдено</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>267515</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>105 678 ₽</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
attempts to make work on mac..
</commit_message>
<xml_diff>
--- a/temp_data.xlsx
+++ b/temp_data.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>87 900 ₽</t>
+          <t>Не найдено</t>
         </is>
       </c>
     </row>
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>105 678 ₽</t>
+          <t>Не найдено</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>87 900 ₽</t>
+          <t>Не найдено</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>105 678 ₽</t>
+          <t>Не найдено</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
non-working aliexpress parser created
</commit_message>
<xml_diff>
--- a/temp_data.xlsx
+++ b/temp_data.xlsx
@@ -7,7 +7,6 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="BonpetData" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -432,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -449,21 +448,11 @@
           <t>АВР-Б-100-2-1</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Не найдено</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>bababab</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Не найдено</t>
         </is>
       </c>
     </row>
@@ -473,69 +462,9 @@
           <t>267515</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Не найдено</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>АВР-Б-100-2-1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Не найдено</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>bababab</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Не найдено</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>267515</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Не найдено</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
working aliexpress scraper + single instance webdriver
</commit_message>
<xml_diff>
--- a/temp_data.xlsx
+++ b/temp_data.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AliexpressData" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -431,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -448,6 +449,56 @@
           <t>АВР-Б-100-2-1</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>9 749 ₽</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>977 ₽</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>6 913,27 ₽</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>750 ₽</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>10 181 ₽</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>1 729 ₽</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>11 835,01 ₽</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>8 092,97 ₽</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>6 710,31 ₽</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>6 152,18 ₽</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -455,11 +506,31 @@
           <t>bababab</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>329 ₽</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>449 ₽</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>146 ₽</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>267515</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Не найдено</t>
         </is>
       </c>
     </row>
@@ -467,4 +538,114 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>АВР-Б-100-2-1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>9 749 ₽</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>977 ₽</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>6 913,27 ₽</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>750 ₽</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>10 181 ₽</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>1 729 ₽</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>11 835,01 ₽</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>8 092,97 ₽</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>6 710,31 ₽</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>6 152,18 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>bababab</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>329 ₽</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>449 ₽</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>146 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>267515</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Не найдено</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
proper 2 ali+bonpet, decent excel
</commit_message>
<xml_diff>
--- a/temp_data.xlsx
+++ b/temp_data.xlsx
@@ -7,7 +7,8 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="AliexpressData" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Bonpet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Aliexpress" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -52,9 +53,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -432,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -444,97 +448,418 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>АВР-Б-100-2-1</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>9 749 ₽</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>977 ₽</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>6 913,27 ₽</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>750 ₽</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>10 181 ₽</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>1 729 ₽</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>11 835,01 ₽</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>8 092,97 ₽</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>6 710,31 ₽</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>6 152,18 ₽</t>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>bababab</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>267515</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>bababab</t>
+          <t>shop</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>329 ₽</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>449 ₽</t>
+          <t>price</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>146 ₽</t>
+          <t>shop</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>shop</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>price</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>267515</t>
+          <t>Bonpet</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Не найдено</t>
+          <t>Шкаф АВР 100А, 2 ввода</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>87 900 ₽</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Женский теплый хиджаб Kallove из хлопка</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>459 ₽</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Bonpet</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Блок АВР CHINT NXZM-125H/4B 4P 100А Icn=50 кА</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>105 678 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Масляный насос 074115105A 074115105B 074115105D для Audi 100 A6 C4 VW Transporter T4 Crafter 2,5 TDI AET APL AVT ACV BBE BJK BJJ, 1 шт.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>4 799 ₽</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>10 шт./лот платок из хлопка и вискозы, длинный шарф, Женский сгорающий хиджаб, шаль, мусульманский головной хиджаб, шарф</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2 269 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Регулятор напряжения R438</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3 649 ₽</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Кухонный фартук Eid Mubarak из хлопка и льна</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>439 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>5-100 шт., микроконтроллеры семьи ATmega48, TQFP32 8 бит MCU AVR ATmega, микроконтроллеры ATMEGA48PA-AU</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>9 984 ₽</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Женский теплый хиджаб Kallove из хлопка</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>459 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Sx460 Avr Stamford заводской генератор автоматический регулятор напряжения стабилизатор дизельного электрического двигателя плата управления</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>902 ₽</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>10 шт./лот платок из хлопка и вискозы, длинный шарф, Женский сгорающий хиджаб, шаль, мусульманский головной хиджаб, шарф</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2 269 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1/2 ~ 100/200 шт. I2C RTC DS1307 24C32 модуль часов реального времени AVR ARM PIC крошечный модуль памяти без батареи</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>9 562 ₽</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Кухонный фартук Eid Mubarak из хлопка и льна</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>439 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Модуль AVR для генератора Stamford AS540</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2 092 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5/10/100 шт ATTINY13A-SSUR SOIC-8 оригинальная микросхема 8-разрядный микроконтроллер - MCU RoHS Core AVR Программная память 1 Кбайт Напряжение 5,5 В</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>6 753,69 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5/10/100 шт ATTINY816-MNR VQFN-20 оригинальная микросхема ic 8-разрядный микроконтроллер - MCU RoHS Core AVR Программная память 8 Кбайт Напряжение 5,5 В</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>7 906,16 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ЖК-модуль IIC/I2C 1602 с последовательной синей подсветкой для Arduino 2560 AVR A004</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>19 482 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1/5/10шт ATMEGA2560-16AU TQFP-100 8-разрядный микроконтроллер -MCU RoHS Core AVR Объем оперативной памяти 8 Кбайт 86 входов/выходов Напряжение 5,5 В</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>11 561,83 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Лидер продажOEM/ODM производство многофункциональный встроенный усилитель HI-FI 100 Вт * 2 Bluetooth 5,0 цифровой плеер усилитель USB аудио</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>182 232 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5/10/100 шт ATTINY1616-MNR QFN-20 Оригинальная микросхема 8-разрядного микроконтроллера -MCU RoHS Core AVR 18 с напряжением ввода-вывода 5,5 В</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>6 010,17 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Aliexpress</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5/10/100 шт ATTINY13A-SSU SOIC-8 8-разрядный микроконтроллер -MCU RoHS AVR Data RAM 64 B 6 Напряжение питания ввода-вывода: 5,5 В</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>6 555,42 ₽</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -546,7 +871,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,97 +880,371 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>АВР-Б-100-2-1</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>9 749 ₽</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>977 ₽</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>6 913,27 ₽</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>750 ₽</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>10 181 ₽</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>1 729 ₽</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>11 835,01 ₽</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>8 092,97 ₽</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>6 710,31 ₽</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>6 152,18 ₽</t>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>bababab</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>267515</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>bababab</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>329 ₽</t>
+          <t>price</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>449 ₽</t>
+          <t>name</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>146 ₽</t>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>price</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Шкаф АВР 100А, 2 ввода</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>87 900 ₽</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Блок АВР CHINT NXZM-125H/4B 4P 100А Icn=50 кА</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>105 678 ₽</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>АВР-Б-100-2-1</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>bababab</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
           <t>267515</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Масляный насос 074115105A 074115105B 074115105D для Audi 100 A6 C4 VW Transporter T4 Crafter 2,5 TDI AET APL AVT ACV BBE BJK BJJ, 1 шт.</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Не найдено</t>
+          <t>4 799 ₽</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Женский теплый хиджаб Kallove из хлопка</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>459 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Регулятор напряжения R438</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3 649 ₽</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10 шт./лот платок из хлопка и вискозы, длинный шарф, Женский сгорающий хиджаб, шаль, мусульманский головной хиджаб, шарф</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2 269 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>5-100 шт., микроконтроллеры семьи ATmega48, TQFP32 8 бит MCU AVR ATmega, микроконтроллеры ATMEGA48PA-AU</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9 984 ₽</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Кухонный фартук Eid Mubarak из хлопка и льна</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>439 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sx460 Avr Stamford заводской генератор автоматический регулятор напряжения стабилизатор дизельного электрического двигателя плата управления</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>902 ₽</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Женский теплый хиджаб Kallove из хлопка</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>459 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1/2 ~ 100/200 шт. I2C RTC DS1307 24C32 модуль часов реального времени AVR ARM PIC крошечный модуль памяти без батареи</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9 562 ₽</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10 шт./лот платок из хлопка и вискозы, длинный шарф, Женский сгорающий хиджаб, шаль, мусульманский головной хиджаб, шарф</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2 269 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Модуль AVR для генератора Stamford AS540</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2 092 ₽</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Кухонный фартук Eid Mubarak из хлопка и льна</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>439 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5/10/100 шт ATTINY13A-SSUR SOIC-8 оригинальная микросхема 8-разрядный микроконтроллер - MCU RoHS Core AVR Программная память 1 Кбайт Напряжение 5,5 В</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>6 753,69 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>5/10/100 шт ATTINY816-MNR VQFN-20 оригинальная микросхема ic 8-разрядный микроконтроллер - MCU RoHS Core AVR Программная память 8 Кбайт Напряжение 5,5 В</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>7 906,16 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ЖК-модуль IIC/I2C 1602 с последовательной синей подсветкой для Arduino 2560 AVR A004</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>19 482 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1/5/10шт ATMEGA2560-16AU TQFP-100 8-разрядный микроконтроллер -MCU RoHS Core AVR Объем оперативной памяти 8 Кбайт 86 входов/выходов Напряжение 5,5 В</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11 561,83 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Лидер продажOEM/ODM производство многофункциональный встроенный усилитель HI-FI 100 Вт * 2 Bluetooth 5,0 цифровой плеер усилитель USB аудио</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>182 232 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>5/10/100 шт ATTINY1616-MNR QFN-20 Оригинальная микросхема 8-разрядного микроконтроллера -MCU RoHS Core AVR 18 с напряжением ввода-вывода 5,5 В</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>6 010,17 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5/10/100 шт ATTINY13A-SSU SOIC-8 8-разрядный микроконтроллер -MCU RoHS AVR Data RAM 64 B 6 Напряжение питания ввода-вывода: 5,5 В</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>6 555,42 ₽</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>